<commit_message>
Re-arranged for better structure
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Google Drive\Code\Python\extract_COVID19_events_from_Twitter\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Code\Python\extract_COVID19_events_from_Twitter\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7055150E-CE60-4C0D-8970-DEA57E2A03FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8922DBC2-2BEF-4643-8C2F-37E8B53CB60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{09ECAD97-3C1E-45DE-875A-3C5CD2F3C873}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{09ECAD97-3C1E-45DE-875A-3C5CD2F3C873}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="7" r:id="rId1"/>
@@ -1247,7 +1247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1264,6 +1264,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1292,12 +1300,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1616,15 +1626,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>309</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>306</v>
       </c>
@@ -1652,7 +1662,7 @@
         <v>0.59208791208791212</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -1669,7 +1679,7 @@
         <v>0.57496796240922687</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>341</v>
       </c>
@@ -1686,7 +1696,7 @@
         <v>0.62478705281090285</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>340</v>
       </c>
@@ -1703,7 +1713,7 @@
         <v>0.16226708074534163</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -1730,22 +1740,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7C2FD4-A612-48B7-B14F-F3EAA1F8E07F}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.46484375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1781,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1790,11 +1800,11 @@
         <f>bert!$Y2</f>
         <v>0.63414634146341398</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <f>biobert!$Y2</f>
         <v>0.68965517241379304</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f>'covid-twitter-bert'!$Y2</f>
         <v>0.77419354838709598</v>
       </c>
@@ -1803,11 +1813,11 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="2">
@@ -1822,11 +1832,11 @@
         <f>bert!$Y3</f>
         <v>0.34426229508196698</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <f>biobert!$Y3</f>
         <v>0.38961038961038902</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f>'covid-twitter-bert'!$Y3</f>
         <v>0.44615384615384601</v>
       </c>
@@ -1835,11 +1845,11 @@
         <v>0.32258064516128998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="2">
@@ -1867,7 +1877,7 @@
         <v>0.47567567567567498</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1882,7 +1892,7 @@
         <f>'bert-paper'!$Z5</f>
         <v>0.72549019607843102</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <f>bert!$Y5</f>
         <v>0.61751152073732696</v>
       </c>
@@ -1894,12 +1904,12 @@
         <f>'covid-twitter-bert'!$Y5</f>
         <v>0.66412213740458004</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f>electra!$Y5</f>
         <v>0.67346938775510201</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1914,7 +1924,7 @@
         <f>'bert-paper'!$Z6</f>
         <v>0.707317073170731</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <f>bert!$Y6</f>
         <v>0.62222222222222201</v>
       </c>
@@ -1922,7 +1932,7 @@
         <f>biobert!$Y6</f>
         <v>0.5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f>'covid-twitter-bert'!$Y6</f>
         <v>0.6875</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +1960,7 @@
         <f>bert!$Y7</f>
         <v>0.74104401228249706</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <f>biobert!$Y7</f>
         <v>0.74285714285714199</v>
       </c>
@@ -1958,12 +1968,12 @@
         <f>'covid-twitter-bert'!$Y7</f>
         <v>0.76126126126126104</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f>electra!$Y7</f>
         <v>0.76735459662288896</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1978,15 +1988,15 @@
         <f>'bert-paper'!$Z8</f>
         <v>0.5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <f>bert!$Y8</f>
         <v>0.41463414634146301</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <f>biobert!$Y8</f>
         <v>0.41463414634146301</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f>'covid-twitter-bert'!$Y8</f>
         <v>0.452380952380952</v>
       </c>
@@ -1995,7 +2005,7 @@
         <v>0.430379746835443</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2022,16 +2032,16 @@
         <f>'covid-twitter-bert'!$Y9</f>
         <v>0.53333333333333299</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f>electra!$Y9</f>
         <v>0.57142857142857095</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C10" s="2">
@@ -2042,7 +2052,7 @@
         <f>'bert-paper'!$Z10</f>
         <v>0.28125</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <f>bert!$Y10</f>
         <v>0.44827586206896503</v>
       </c>
@@ -2050,7 +2060,7 @@
         <f>biobert!$Y10</f>
         <v>0.4375</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f>'covid-twitter-bert'!$Y10</f>
         <v>0.50909090909090904</v>
       </c>
@@ -2059,7 +2069,7 @@
         <v>0.46153846153846101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2078,7 +2088,7 @@
         <f>bert!$Y11</f>
         <v>0.57142857142857095</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <f>biobert!$Y11</f>
         <v>0.57289002557544699</v>
       </c>
@@ -2086,12 +2096,12 @@
         <f>'covid-twitter-bert'!$Y11</f>
         <v>0.59905660377358405</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f>electra!$Y11</f>
         <v>0.62034739454094201</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -2123,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -2170,7 +2180,7 @@
         <f>'bert-paper'!$Z14</f>
         <v>0.57894736842105199</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <f>bert!$Y14</f>
         <v>0.63829787234042501</v>
       </c>
@@ -2178,7 +2188,7 @@
         <f>biobert!$Y14</f>
         <v>0.42105263157894701</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f>'covid-twitter-bert'!$Y14</f>
         <v>0.65217391304347805</v>
       </c>
@@ -2187,7 +2197,7 @@
         <v>0.59340659340659296</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -2202,7 +2212,7 @@
         <f>'bert-paper'!$Z15</f>
         <v>0.54545454545454497</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <f>bert!$Y15</f>
         <v>0.55000000000000004</v>
       </c>
@@ -2210,7 +2220,7 @@
         <f>biobert!$Y15</f>
         <v>0.41025641025641002</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f>'covid-twitter-bert'!$Y15</f>
         <v>0.60465116279069697</v>
       </c>
@@ -2219,7 +2229,7 @@
         <v>0.58064516129032195</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -2266,7 +2276,7 @@
         <f>'bert-paper'!$Z17</f>
         <v>0.49397590361445698</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <f>bert!$Y17</f>
         <v>0.60586319218241003</v>
       </c>
@@ -2274,7 +2284,7 @@
         <f>biobert!$Y17</f>
         <v>0.55830388692579502</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f>'covid-twitter-bert'!$Y17</f>
         <v>0.68259385665529004</v>
       </c>
@@ -2283,7 +2293,7 @@
         <v>0.65084745762711804</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -2298,7 +2308,7 @@
         <f>'bert-paper'!$Z18</f>
         <v>0.63157894736842102</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="4">
         <f>bert!$Y18</f>
         <v>0.60465116279069697</v>
       </c>
@@ -2306,7 +2316,7 @@
         <f>biobert!$Y18</f>
         <v>0.46511627906976699</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f>'covid-twitter-bert'!$Y18</f>
         <v>0.71111111111111103</v>
       </c>
@@ -2315,7 +2325,7 @@
         <v>0.62222222222222201</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -2347,7 +2357,7 @@
         <v>0.16666666666666599</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -2366,7 +2376,7 @@
         <f>bert!$Y20</f>
         <v>0.375</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="4">
         <f>biobert!$Y20</f>
         <v>0.42857142857142799</v>
       </c>
@@ -2374,12 +2384,12 @@
         <f>'covid-twitter-bert'!$Y20</f>
         <v>0.439024390243902</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f>electra!$Y20</f>
         <v>0.45714285714285702</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2398,11 +2408,11 @@
         <f>bert!$Y21</f>
         <v>0.50476190476190397</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <f>biobert!$Y21</f>
         <v>0.54634146341463397</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f>'covid-twitter-bert'!$Y21</f>
         <v>0.57261410788381695</v>
       </c>
@@ -2411,7 +2421,7 @@
         <v>0.56410256410256399</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2443,7 +2453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -2458,7 +2468,7 @@
         <f>'bert-paper'!$Z23</f>
         <v>0.49275362318840499</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4">
         <f>bert!$Y23</f>
         <v>0.55855855855855796</v>
       </c>
@@ -2466,7 +2476,7 @@
         <f>biobert!$Y23</f>
         <v>0.54716981132075404</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f>'covid-twitter-bert'!$Y23</f>
         <v>0.57999999999999996</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>0.507692307692307</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2490,15 +2500,15 @@
         <f>'bert-paper'!$Z24</f>
         <v>0.53846153846153799</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <f>bert!$Y24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="4">
         <f>biobert!$Y24</f>
         <v>0</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f>'covid-twitter-bert'!$Y24</f>
         <v>0.46153846153846101</v>
       </c>
@@ -2507,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -2526,11 +2536,11 @@
         <f>bert!$Y25</f>
         <v>0.52307692307692299</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="4">
         <f>biobert!$Y25</f>
         <v>0.537313432835821</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f>'covid-twitter-bert'!$Y25</f>
         <v>0.64</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>0.61971830985915499</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -2558,7 +2568,7 @@
         <f>bert!$Y26</f>
         <v>0.75</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="4">
         <f>biobert!$Y26</f>
         <v>0.76923076923076905</v>
       </c>
@@ -2566,12 +2576,12 @@
         <f>'covid-twitter-bert'!$Y26</f>
         <v>0.73015873015873001</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <f>electra!$Y26</f>
         <v>0.80645161290322498</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -2586,7 +2596,7 @@
         <f>'bert-paper'!$Z27</f>
         <v>0.57142857142857095</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <f>bert!$Y27</f>
         <v>0.66867469879518004</v>
       </c>
@@ -2598,12 +2608,12 @@
         <f>'covid-twitter-bert'!$Y27</f>
         <v>0.69648562300319405</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <f>electra!$Y27</f>
         <v>0.70503597122302097</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -2618,7 +2628,7 @@
         <f>'bert-paper'!$Z28</f>
         <v>0</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="4">
         <f>bert!$Y28</f>
         <v>0.63636363636363602</v>
       </c>
@@ -2626,7 +2636,7 @@
         <f>biobert!$Y28</f>
         <v>0.43243243243243201</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f>'covid-twitter-bert'!$Y28</f>
         <v>0.65116279069767402</v>
       </c>
@@ -2635,7 +2645,7 @@
         <v>0.42857142857142799</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -2686,11 +2696,11 @@
         <f>bert!$Y30</f>
         <v>0.59770114942528696</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="4">
         <f>biobert!$Y30</f>
         <v>0.63736263736263699</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <f>'covid-twitter-bert'!$Y30</f>
         <v>0.65060240963855398</v>
       </c>
@@ -2699,7 +2709,7 @@
         <v>0.57534246575342396</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -2714,7 +2724,7 @@
         <f>'bert-paper'!$Z31</f>
         <v>0.371428571428571</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="4">
         <f>bert!$Y31</f>
         <v>0.61870503597122295</v>
       </c>
@@ -2726,12 +2736,12 @@
         <f>'covid-twitter-bert'!$Y31</f>
         <v>0.63888888888888895</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <f>electra!$Y31</f>
         <v>0.67272727272727195</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -2750,11 +2760,11 @@
         <f>bert!$Y32</f>
         <v>0.47368421052631499</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="4">
         <f>biobert!$Y32</f>
         <v>0.475728155339805</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <f>'covid-twitter-bert'!$Y32</f>
         <v>0.54666666666666597</v>
       </c>
@@ -2763,7 +2773,7 @@
         <v>0.52112676056338003</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -2778,7 +2788,7 @@
         <f>'bert-paper'!$Z33</f>
         <v>0.30392156862745001</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="4">
         <f>bert!$Y33</f>
         <v>0.61702127659574402</v>
       </c>
@@ -2790,12 +2800,12 @@
         <f>'covid-twitter-bert'!$Y33</f>
         <v>0.61052631578947303</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <f>electra!$Y33</f>
         <v>0.66425992779783305</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -2810,7 +2820,7 @@
         <f>'bert-paper'!$Z34</f>
         <v>0</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <f>bert!$Y34</f>
         <v>0.44776119402984998</v>
       </c>
@@ -2818,7 +2828,7 @@
         <f>biobert!$Y34</f>
         <v>0.42231075697211101</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <f>'covid-twitter-bert'!$Y34</f>
         <v>0.520231213872832</v>
       </c>
@@ -2836,20 +2846,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645B2E46-A973-4F43-A440-0DFDA26D52C4}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="24" width="9.06640625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="1"/>
-    <col min="26" max="30" width="9.06640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="24" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="9.109375" style="1"/>
+    <col min="26" max="30" width="9.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2950,7 +2960,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3054,7 +3064,7 @@
         <v>0.59208791208791212</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3127,7 +3137,7 @@
       <c r="X3">
         <v>62</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="5">
         <v>0.34426229508196698</v>
       </c>
       <c r="Z3">
@@ -3146,7 +3156,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3219,7 +3229,7 @@
       <c r="X4">
         <v>103</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="5">
         <v>0.480392156862745</v>
       </c>
       <c r="Z4">
@@ -3238,7 +3248,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -3330,7 +3340,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3422,7 +3432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -3514,7 +3524,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3606,7 +3616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3698,7 +3708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -3790,7 +3800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3882,7 +3892,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -3974,7 +3984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -4158,7 +4168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -4250,7 +4260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -4342,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -4434,7 +4444,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -4526,7 +4536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -4618,7 +4628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -4710,7 +4720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -4802,7 +4812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -4894,7 +4904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -4986,7 +4996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -5078,7 +5088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -5170,7 +5180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -5262,7 +5272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -5354,7 +5364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -5446,7 +5456,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -5538,7 +5548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -5630,7 +5640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -5722,7 +5732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -5814,7 +5824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -5906,7 +5916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -6000,6 +6010,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6011,16 +6022,16 @@
       <selection activeCell="AE1" sqref="AE1:AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="24" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.265625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.21875" style="1" customWidth="1"/>
     <col min="26" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6121,7 +6132,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -6225,7 +6236,7 @@
         <v>0.57496796240922687</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6317,7 +6328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -6409,7 +6420,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -6501,7 +6512,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -6593,7 +6604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -6685,7 +6696,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -6777,7 +6788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -6869,7 +6880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -6961,7 +6972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -7053,7 +7064,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -7145,7 +7156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -7237,7 +7248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -7329,7 +7340,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -7421,7 +7432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -7513,7 +7524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -7605,7 +7616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -7697,7 +7708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -7789,7 +7800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -7881,7 +7892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -7973,7 +7984,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -8065,7 +8076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -8157,7 +8168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -8249,7 +8260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -8341,7 +8352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -8433,7 +8444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -8525,7 +8536,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -8617,7 +8628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -8709,7 +8720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -8801,7 +8812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -8893,7 +8904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -8985,7 +8996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -9077,7 +9088,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -9178,20 +9189,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40168F0E-FC16-4362-B18F-2CE5356F0709}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="24" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="1"/>
+    <col min="25" max="25" width="9.109375" style="1"/>
     <col min="26" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9292,7 +9303,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -9396,7 +9407,7 @@
         <v>0.63035714285714284</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -9488,7 +9499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -9580,7 +9591,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -9672,7 +9683,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -9764,7 +9775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -9856,7 +9867,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -9948,7 +9959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -10040,7 +10051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -10132,7 +10143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -10224,7 +10235,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -10316,7 +10327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -10408,7 +10419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -10500,7 +10511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -10592,7 +10603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -10684,7 +10695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -10776,7 +10787,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -10868,7 +10879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -10960,7 +10971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -11052,7 +11063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -11144,7 +11155,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -11236,7 +11247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -11328,7 +11339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -11420,7 +11431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -11512,7 +11523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -11604,7 +11615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -11696,7 +11707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -11788,7 +11799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -11880,7 +11891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -11972,7 +11983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -12064,7 +12075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -12156,7 +12167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -12248,7 +12259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -12350,19 +12361,19 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AG2"/>
+      <selection activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="24" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="1"/>
+    <col min="25" max="25" width="9.109375" style="1"/>
     <col min="26" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12463,7 +12474,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -12567,7 +12578,7 @@
         <v>0.62478705281090285</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -12659,7 +12670,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -12751,7 +12762,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -12843,7 +12854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -12935,7 +12946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -13027,7 +13038,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -13119,7 +13130,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -13211,7 +13222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -13303,7 +13314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -13395,7 +13406,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -13487,7 +13498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -13579,7 +13590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -13671,7 +13682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -13763,7 +13774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -13855,7 +13866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -13947,7 +13958,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -14039,7 +14050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -14131,7 +14142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -14223,7 +14234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -14315,7 +14326,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -14407,7 +14418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -14499,7 +14510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -14591,7 +14602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -14683,7 +14694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -14775,7 +14786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -14867,7 +14878,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -14959,7 +14970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -15051,7 +15062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -15143,7 +15154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -15235,7 +15246,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -15327,7 +15338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -15419,7 +15430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -15520,19 +15531,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DB2610-41A0-4FBA-A977-EFC7065CE8F3}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="24" width="0" hidden="1" customWidth="1"/>
     <col min="26" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15633,7 +15644,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -15737,7 +15748,7 @@
         <v>0.16226708074534163</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -15829,7 +15840,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -15921,7 +15932,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -16013,7 +16024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -16105,7 +16116,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -16197,7 +16208,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -16289,7 +16300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -16381,7 +16392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -16473,7 +16484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -16565,7 +16576,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -16657,7 +16668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -16749,7 +16760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -16841,7 +16852,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -16933,7 +16944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -17025,7 +17036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -17117,7 +17128,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -17209,7 +17220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -17301,7 +17312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -17393,7 +17404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -17485,7 +17496,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -17577,7 +17588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -17669,7 +17680,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -17761,7 +17772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -17853,7 +17864,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -17945,7 +17956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -18037,7 +18048,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -18129,7 +18140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -18221,7 +18232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -18313,7 +18324,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -18405,7 +18416,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -18497,7 +18508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -18589,7 +18600,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -18694,17 +18705,17 @@
       <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="25" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.06640625" style="1"/>
+    <col min="26" max="26" width="9.109375" style="1"/>
     <col min="27" max="28" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18799,7 +18810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -18894,7 +18905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -18989,7 +19000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -19084,7 +19095,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -19179,7 +19190,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -19274,7 +19285,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -19369,7 +19380,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -19464,7 +19475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -19559,7 +19570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -19654,7 +19665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -19749,7 +19760,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -19844,7 +19855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -19939,7 +19950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -20034,7 +20045,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -20129,7 +20140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -20224,7 +20235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -20319,7 +20330,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -20414,7 +20425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -20509,7 +20520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -20604,7 +20615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -20699,7 +20710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -20794,7 +20805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -20889,7 +20900,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -20984,7 +20995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -21079,7 +21090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -21174,7 +21185,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -21269,7 +21280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -21364,7 +21375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -21459,7 +21470,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -21554,7 +21565,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -21649,7 +21660,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -21744,7 +21755,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -21839,7 +21850,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>
@@ -21933,17 +21944,17 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="24" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="1"/>
+    <col min="25" max="25" width="9.109375" style="1"/>
     <col min="26" max="27" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -22035,7 +22046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -22127,7 +22138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -22219,7 +22230,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -22311,7 +22322,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -22403,7 +22414,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -22495,7 +22506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -22587,7 +22598,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -22679,7 +22690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -22771,7 +22782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -22863,7 +22874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -22955,7 +22966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -23047,7 +23058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -23139,7 +23150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -23231,7 +23242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -23323,7 +23334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -23415,7 +23426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -23507,7 +23518,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -23599,7 +23610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -23691,7 +23702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -23783,7 +23794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -23875,7 +23886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -23967,7 +23978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -24059,7 +24070,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -24085,7 +24096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -24177,7 +24188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -24269,7 +24280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -24361,7 +24372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -24453,7 +24464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -24545,7 +24556,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -24637,7 +24648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -24729,7 +24740,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -24821,7 +24832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -24913,7 +24924,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>160</v>
       </c>

</xml_diff>